<commit_message>
Work Orders Validated and Processed
</commit_message>
<xml_diff>
--- a/src/Files/160A110V.xlsx
+++ b/src/Files/160A110V.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\WORK ORDERS\160A\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luke\eclipse-workspace\BURIN_V2\src\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="75" windowWidth="3120" windowHeight="8775"/>
+    <workbookView xWindow="6000" yWindow="78" windowWidth="3120" windowHeight="8778"/>
   </bookViews>
   <sheets>
     <sheet name="160-A WO" sheetId="8" r:id="rId1"/>
@@ -333,7 +333,7 @@
     <t>160A</t>
   </si>
   <si>
-    <t>DO NOT KIT - Hoa's FLOOR STOCK</t>
+    <t>FLOOR STOCK</t>
   </si>
 </sst>
 </file>
@@ -973,25 +973,25 @@
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="31.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="7.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="31.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.71875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.71875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="9.71875" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="14.1" x14ac:dyDescent="0.5">
       <c r="A1" s="64" t="s">
         <v>93</v>
       </c>
@@ -1011,7 +1011,7 @@
       <c r="I1" s="9"/>
       <c r="J1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="13.8" x14ac:dyDescent="0.45">
       <c r="A2" s="67" t="s">
         <v>83</v>
       </c>
@@ -1031,7 +1031,7 @@
       <c r="I2" s="12"/>
       <c r="J2" s="13"/>
     </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="14.1" x14ac:dyDescent="0.5">
       <c r="A3" s="14"/>
       <c r="B3" s="15"/>
       <c r="C3" s="16">
@@ -1051,7 +1051,7 @@
       <c r="I3" s="18"/>
       <c r="J3" s="13"/>
     </row>
-    <row r="4" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="14"/>
       <c r="B4" s="19"/>
       <c r="C4" s="20" t="s">
@@ -1067,7 +1067,7 @@
       <c r="I4" s="22"/>
       <c r="J4" s="13"/>
     </row>
-    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="14.1" x14ac:dyDescent="0.5">
       <c r="A5" s="23"/>
       <c r="B5" s="19"/>
       <c r="C5" s="24" t="s">
@@ -1083,7 +1083,7 @@
       <c r="I5" s="22"/>
       <c r="J5" s="13"/>
     </row>
-    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="14"/>
       <c r="B6" s="19"/>
       <c r="C6" s="25" t="s">
@@ -1097,7 +1097,7 @@
       <c r="I6" s="26"/>
       <c r="J6" s="13"/>
     </row>
-    <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="14"/>
       <c r="B7" s="19"/>
       <c r="C7" s="26"/>
@@ -1109,7 +1109,7 @@
       <c r="I7" s="26"/>
       <c r="J7" s="13"/>
     </row>
-    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="14.1" x14ac:dyDescent="0.5">
       <c r="A8" s="28" t="s">
         <v>101</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="58">
         <v>5200</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>4.29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="58">
         <v>5202</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>1.29</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="58">
         <v>5349</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="58">
         <v>5352</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="7" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" s="7" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="58">
         <v>6244</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>58.199999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="7" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" s="7" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="58">
         <v>6245</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>0.21000000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="7" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" s="7" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="58">
         <v>6431</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>0.21000000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="6" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" s="6" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="58">
         <v>6434</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="58">
         <v>6466</v>
       </c>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="J17" s="49"/>
     </row>
-    <row r="18" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="58">
         <v>6546</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>18.240000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="58">
         <v>6588</v>
       </c>
@@ -1445,7 +1445,7 @@
       </c>
       <c r="J19" s="49"/>
     </row>
-    <row r="20" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="14"/>
       <c r="B20" s="55"/>
       <c r="C20" s="55"/>
@@ -1457,7 +1457,7 @@
       <c r="I20" s="54"/>
       <c r="J20" s="13"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A21" s="62" t="s">
         <v>104</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="I21" s="54"/>
       <c r="J21" s="13"/>
     </row>
-    <row r="22" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="58">
         <v>5004</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="58">
         <v>5012</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="58">
         <v>5015</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="58">
         <v>5080</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="58">
         <v>5077</v>
       </c>
@@ -1607,7 +1607,7 @@
       <c r="I26" s="43"/>
       <c r="J26" s="38"/>
     </row>
-    <row r="27" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="58">
         <v>5089</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="58">
         <v>5301</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="58">
         <v>5307</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="58">
         <v>5310</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="58">
         <v>5311</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="58">
         <v>5313</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="58">
         <v>5315</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="58">
         <v>5318</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="58">
         <v>5321</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="58">
         <v>5323</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="58">
         <v>5324</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="58">
         <v>5328</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="58">
         <v>5338</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="58">
         <v>5339</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="58">
         <v>5340</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="58">
         <v>5341</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="58">
         <v>5342</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="58">
         <v>5343</v>
       </c>

</xml_diff>

<commit_message>
START and END row enforcement
</commit_message>
<xml_diff>
--- a/src/Files/160A110V.xlsx
+++ b/src/Files/160A110V.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="107">
   <si>
     <t>QTY</t>
   </si>
@@ -334,6 +334,12 @@
   </si>
   <si>
     <t>FLOOR STOCK</t>
+  </si>
+  <si>
+    <t>START</t>
+  </si>
+  <si>
+    <t>END</t>
   </si>
 </sst>
 </file>
@@ -970,10 +976,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -1141,39 +1147,23 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="58">
-        <v>5200</v>
-      </c>
-      <c r="B9" s="39">
-        <v>1</v>
-      </c>
-      <c r="C9" s="33">
-        <f>SUM(B9*C3)</f>
-        <v>3</v>
-      </c>
-      <c r="D9" s="40"/>
-      <c r="E9" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="G9" s="40"/>
-      <c r="H9" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="I9" s="45">
-        <v>1.43</v>
-      </c>
-      <c r="J9" s="38">
-        <f t="shared" ref="J9:J16" si="0">I9*C9</f>
-        <v>4.29</v>
-      </c>
+    <row r="9" spans="1:10" ht="14.1" x14ac:dyDescent="0.5">
+      <c r="A9" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="32"/>
     </row>
     <row r="10" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="58">
-        <v>5202</v>
+        <v>5200</v>
       </c>
       <c r="B10" s="39">
         <v>1</v>
@@ -1183,29 +1173,27 @@
         <v>3</v>
       </c>
       <c r="D10" s="40"/>
-      <c r="E10" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="G10" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="H10" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="I10" s="43">
-        <v>0.43</v>
+      <c r="E10" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" s="40"/>
+      <c r="H10" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="I10" s="45">
+        <v>1.43</v>
       </c>
       <c r="J10" s="38">
-        <f t="shared" si="0"/>
-        <v>1.29</v>
+        <f t="shared" ref="J10:J17" si="0">I10*C10</f>
+        <v>4.29</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="58">
-        <v>5349</v>
+        <v>5202</v>
       </c>
       <c r="B11" s="39">
         <v>1</v>
@@ -1215,29 +1203,29 @@
         <v>3</v>
       </c>
       <c r="D11" s="40"/>
-      <c r="E11" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="F11" s="41" t="s">
-        <v>88</v>
+      <c r="E11" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>70</v>
       </c>
       <c r="G11" s="42" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="H11" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="52">
-        <v>76</v>
+        <v>47</v>
+      </c>
+      <c r="I11" s="43">
+        <v>0.43</v>
       </c>
       <c r="J11" s="38">
         <f t="shared" si="0"/>
-        <v>228</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="58">
-        <v>5352</v>
+        <v>5349</v>
       </c>
       <c r="B12" s="39">
         <v>1</v>
@@ -1248,10 +1236,10 @@
       </c>
       <c r="D12" s="40"/>
       <c r="E12" s="41" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="F12" s="41" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="G12" s="42" t="s">
         <v>42</v>
@@ -1260,42 +1248,48 @@
         <v>43</v>
       </c>
       <c r="I12" s="52">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="J12" s="38">
         <f t="shared" si="0"/>
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="7" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="58">
-        <v>6244</v>
-      </c>
-      <c r="B13" s="33">
+        <v>5352</v>
+      </c>
+      <c r="B13" s="39">
         <v>1</v>
       </c>
       <c r="C13" s="33">
         <f>SUM(B13*C3)</f>
         <v>3</v>
       </c>
-      <c r="D13" s="33"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="50"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="43">
-        <v>19.399999999999999</v>
-      </c>
-      <c r="J13" s="53">
+      <c r="D13" s="40"/>
+      <c r="E13" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" s="52">
+        <v>39</v>
+      </c>
+      <c r="J13" s="38">
         <f t="shared" si="0"/>
-        <v>58.199999999999996</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="7" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="58">
-        <v>6245</v>
+        <v>6244</v>
       </c>
       <c r="B14" s="33">
         <v>1</v>
@@ -1307,21 +1301,21 @@
       <c r="D14" s="33"/>
       <c r="E14" s="50"/>
       <c r="F14" s="47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G14" s="50"/>
       <c r="H14" s="50"/>
       <c r="I14" s="43">
-        <v>7.0000000000000007E-2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="J14" s="53">
         <f t="shared" si="0"/>
-        <v>0.21000000000000002</v>
+        <v>58.199999999999996</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="7" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="58">
-        <v>6431</v>
+        <v>6245</v>
       </c>
       <c r="B15" s="33">
         <v>1</v>
@@ -1330,13 +1324,13 @@
         <f>SUM(B15*C3)</f>
         <v>3</v>
       </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="48" t="s">
-        <v>78</v>
+      <c r="D15" s="33"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="47" t="s">
+        <v>52</v>
       </c>
       <c r="G15" s="50"/>
-      <c r="H15" s="37"/>
+      <c r="H15" s="50"/>
       <c r="I15" s="43">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -1345,58 +1339,61 @@
         <v>0.21000000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="6" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" s="7" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="58">
-        <v>6434</v>
+        <v>6431</v>
       </c>
       <c r="B16" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" s="33">
         <f>SUM(B16*C3)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D16" s="34"/>
       <c r="E16" s="51"/>
       <c r="F16" s="48" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G16" s="50"/>
       <c r="H16" s="37"/>
       <c r="I16" s="43">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="J16" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
+        <v>0.21000000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="6" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="58">
-        <v>6466</v>
+        <v>6434</v>
       </c>
       <c r="B17" s="33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" s="33">
         <f>SUM(B17*C3)</f>
-        <v>3</v>
-      </c>
-      <c r="D17" s="33"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="47" t="s">
-        <v>86</v>
+        <v>6</v>
+      </c>
+      <c r="D17" s="34"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="48" t="s">
+        <v>77</v>
       </c>
       <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
+      <c r="H17" s="37"/>
       <c r="I17" s="43">
-        <v>1</v>
-      </c>
-      <c r="J17" s="49"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="53">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="58">
-        <v>6546</v>
+        <v>6466</v>
       </c>
       <c r="B18" s="33">
         <v>1</v>
@@ -1405,26 +1402,21 @@
         <f>SUM(B18*C3)</f>
         <v>3</v>
       </c>
-      <c r="D18" s="34"/>
-      <c r="E18" s="51" t="s">
-        <v>94</v>
-      </c>
-      <c r="F18" s="48" t="s">
-        <v>85</v>
+      <c r="D18" s="33"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="47" t="s">
+        <v>86</v>
       </c>
       <c r="G18" s="50"/>
-      <c r="H18" s="37"/>
+      <c r="H18" s="50"/>
       <c r="I18" s="43">
-        <v>6.08</v>
-      </c>
-      <c r="J18" s="38">
-        <f>I18*C18</f>
-        <v>18.240000000000002</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="58">
-        <v>6588</v>
+        <v>6546</v>
       </c>
       <c r="B19" s="33">
         <v>1</v>
@@ -1434,93 +1426,96 @@
         <v>3</v>
       </c>
       <c r="D19" s="34"/>
-      <c r="E19" s="51"/>
+      <c r="E19" s="51" t="s">
+        <v>94</v>
+      </c>
       <c r="F19" s="48" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="G19" s="50"/>
       <c r="H19" s="37"/>
       <c r="I19" s="43">
-        <v>1</v>
-      </c>
-      <c r="J19" s="49"/>
-    </row>
-    <row r="20" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="14"/>
-      <c r="B20" s="55"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="54"/>
-      <c r="J20" s="13"/>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="62" t="s">
-        <v>104</v>
-      </c>
-      <c r="B21" s="63"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
+        <v>6.08</v>
+      </c>
+      <c r="J19" s="38">
+        <f>I19*C19</f>
+        <v>18.240000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="58">
+        <v>6588</v>
+      </c>
+      <c r="B20" s="33">
+        <v>1</v>
+      </c>
+      <c r="C20" s="33">
+        <f>SUM(B20*C3)</f>
+        <v>3</v>
+      </c>
+      <c r="D20" s="34"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="50"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="43">
+        <v>1</v>
+      </c>
+      <c r="J20" s="49"/>
+    </row>
+    <row r="21" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" s="55"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
       <c r="E21" s="13"/>
       <c r="F21" s="56"/>
-      <c r="G21" s="57"/>
+      <c r="G21" s="56"/>
       <c r="H21" s="56"/>
       <c r="I21" s="54"/>
       <c r="J21" s="13"/>
     </row>
-    <row r="22" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="58">
-        <v>5004</v>
-      </c>
-      <c r="B22" s="33">
-        <v>1</v>
-      </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="F22" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="G22" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="H22" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="I22" s="38">
-        <v>25.38</v>
-      </c>
-      <c r="J22" s="38">
-        <f>I22*C22</f>
-        <v>0</v>
-      </c>
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A22" s="62" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" s="63"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="13"/>
     </row>
     <row r="23" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="58">
-        <v>5012</v>
-      </c>
-      <c r="B23" s="39">
+        <v>5004</v>
+      </c>
+      <c r="B23" s="33">
         <v>1</v>
       </c>
       <c r="C23" s="33"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="35">
-        <v>2860124541</v>
-      </c>
-      <c r="F23" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="I23" s="43">
-        <v>10.06</v>
+      <c r="D23" s="34"/>
+      <c r="E23" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="G23" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="H23" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="I23" s="38">
+        <v>25.38</v>
       </c>
       <c r="J23" s="38">
         <f>I23*C23</f>
@@ -1529,25 +1524,25 @@
     </row>
     <row r="24" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="58">
-        <v>5015</v>
+        <v>5012</v>
       </c>
       <c r="B24" s="39">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C24" s="33"/>
       <c r="D24" s="40"/>
       <c r="E24" s="35">
-        <v>2860133353</v>
+        <v>2860124541</v>
       </c>
       <c r="F24" s="35" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G24" s="42"/>
       <c r="H24" s="42" t="s">
         <v>28</v>
       </c>
       <c r="I24" s="43">
-        <v>0.27</v>
+        <v>10.06</v>
       </c>
       <c r="J24" s="38">
         <f>I24*C24</f>
@@ -1556,27 +1551,25 @@
     </row>
     <row r="25" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="58">
-        <v>5080</v>
-      </c>
-      <c r="B25" s="33">
-        <v>2</v>
+        <v>5015</v>
+      </c>
+      <c r="B25" s="39">
+        <v>4</v>
       </c>
       <c r="C25" s="33"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="G25" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="H25" s="37" t="s">
-        <v>12</v>
+      <c r="D25" s="40"/>
+      <c r="E25" s="35">
+        <v>2860133353</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42" t="s">
+        <v>28</v>
       </c>
       <c r="I25" s="43">
-        <v>25.58</v>
+        <v>0.27</v>
       </c>
       <c r="J25" s="38">
         <f>I25*C25</f>
@@ -1585,105 +1578,107 @@
     </row>
     <row r="26" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="58">
-        <v>5077</v>
-      </c>
-      <c r="B26" s="39">
-        <v>1</v>
+        <v>5080</v>
+      </c>
+      <c r="B26" s="33">
+        <v>2</v>
       </c>
       <c r="C26" s="33"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="F26" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="G26" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="H26" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="I26" s="43"/>
-      <c r="J26" s="38"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="G26" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="H26" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="I26" s="43">
+        <v>25.58</v>
+      </c>
+      <c r="J26" s="38">
+        <f>I26*C26</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="58">
-        <v>5089</v>
+        <v>5077</v>
       </c>
       <c r="B27" s="39">
         <v>1</v>
       </c>
       <c r="C27" s="33"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="F27" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="I27" s="43">
-        <v>99</v>
-      </c>
-      <c r="J27" s="38">
-        <f t="shared" ref="J27:J44" si="1">I27*C27</f>
-        <v>0</v>
-      </c>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="H27" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="I27" s="43"/>
+      <c r="J27" s="38"/>
     </row>
     <row r="28" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="58">
-        <v>5301</v>
-      </c>
-      <c r="B28" s="33">
+        <v>5089</v>
+      </c>
+      <c r="B28" s="39">
         <v>1</v>
       </c>
       <c r="C28" s="33"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="G28" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="H28" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="I28" s="45">
-        <v>2.66</v>
+      <c r="D28" s="40"/>
+      <c r="E28" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="I28" s="43">
+        <v>99</v>
       </c>
       <c r="J28" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J28:J45" si="1">I28*C28</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="58">
-        <v>5307</v>
-      </c>
-      <c r="B29" s="39">
+        <v>5301</v>
+      </c>
+      <c r="B29" s="33">
         <v>1</v>
       </c>
       <c r="C29" s="33"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="F29" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="G29" s="42"/>
-      <c r="H29" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="I29" s="43">
-        <v>12.2</v>
+      <c r="D29" s="34"/>
+      <c r="E29" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="I29" s="45">
+        <v>2.66</v>
       </c>
       <c r="J29" s="38">
         <f t="shared" si="1"/>
@@ -1692,27 +1687,25 @@
     </row>
     <row r="30" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="58">
-        <v>5310</v>
-      </c>
-      <c r="B30" s="33">
-        <v>6</v>
+        <v>5307</v>
+      </c>
+      <c r="B30" s="39">
+        <v>1</v>
       </c>
       <c r="C30" s="33"/>
-      <c r="D30" s="34"/>
+      <c r="D30" s="40"/>
       <c r="E30" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="G30" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="H30" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="I30" s="49">
-        <v>1.2</v>
+        <v>64</v>
+      </c>
+      <c r="F30" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="I30" s="43">
+        <v>12.2</v>
       </c>
       <c r="J30" s="38">
         <f t="shared" si="1"/>
@@ -1721,27 +1714,27 @@
     </row>
     <row r="31" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="58">
-        <v>5311</v>
+        <v>5310</v>
       </c>
       <c r="B31" s="33">
         <v>6</v>
       </c>
       <c r="C31" s="33"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="F31" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="G31" s="48" t="s">
-        <v>20</v>
+      <c r="E31" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="37" t="s">
+        <v>11</v>
       </c>
       <c r="H31" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I31" s="45">
-        <v>1.05</v>
+      <c r="I31" s="49">
+        <v>1.2</v>
       </c>
       <c r="J31" s="38">
         <f t="shared" si="1"/>
@@ -1750,27 +1743,27 @@
     </row>
     <row r="32" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="58">
-        <v>5313</v>
+        <v>5311</v>
       </c>
       <c r="B32" s="33">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C32" s="33"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="F32" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="G32" s="37" t="s">
+      <c r="E32" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="48" t="s">
         <v>20</v>
       </c>
       <c r="H32" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I32" s="49">
-        <v>1.4</v>
+      <c r="I32" s="45">
+        <v>1.05</v>
       </c>
       <c r="J32" s="38">
         <f t="shared" si="1"/>
@@ -1779,27 +1772,27 @@
     </row>
     <row r="33" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="58">
-        <v>5315</v>
-      </c>
-      <c r="B33" s="39">
+        <v>5313</v>
+      </c>
+      <c r="B33" s="33">
         <v>1</v>
       </c>
       <c r="C33" s="33"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="F33" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="G33" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="H33" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="I33" s="43">
-        <v>2.97</v>
+      <c r="D33" s="34"/>
+      <c r="E33" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="I33" s="49">
+        <v>1.4</v>
       </c>
       <c r="J33" s="38">
         <f t="shared" si="1"/>
@@ -1808,27 +1801,27 @@
     </row>
     <row r="34" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="58">
-        <v>5318</v>
-      </c>
-      <c r="B34" s="33">
+        <v>5315</v>
+      </c>
+      <c r="B34" s="39">
         <v>1</v>
       </c>
       <c r="C34" s="33"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="F34" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="G34" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H34" s="48" t="s">
-        <v>12</v>
+      <c r="D34" s="40"/>
+      <c r="E34" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="F34" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="G34" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="H34" s="35" t="s">
+        <v>75</v>
       </c>
       <c r="I34" s="43">
-        <v>6.9</v>
+        <v>2.97</v>
       </c>
       <c r="J34" s="38">
         <f t="shared" si="1"/>
@@ -1837,27 +1830,27 @@
     </row>
     <row r="35" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="58">
-        <v>5321</v>
+        <v>5318</v>
       </c>
       <c r="B35" s="33">
         <v>1</v>
       </c>
       <c r="C35" s="33"/>
       <c r="D35" s="34"/>
-      <c r="E35" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="F35" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="G35" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="H35" s="37" t="s">
+      <c r="E35" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H35" s="48" t="s">
         <v>12</v>
       </c>
       <c r="I35" s="43">
-        <v>1.06</v>
+        <v>6.9</v>
       </c>
       <c r="J35" s="38">
         <f t="shared" si="1"/>
@@ -1866,27 +1859,27 @@
     </row>
     <row r="36" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="58">
-        <v>5323</v>
+        <v>5321</v>
       </c>
       <c r="B36" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C36" s="33"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="46" t="s">
-        <v>57</v>
-      </c>
-      <c r="F36" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="G36" s="48" t="s">
+      <c r="E36" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="G36" s="36" t="s">
         <v>11</v>
       </c>
       <c r="H36" s="37" t="s">
         <v>12</v>
       </c>
       <c r="I36" s="43">
-        <v>14.7</v>
+        <v>1.06</v>
       </c>
       <c r="J36" s="38">
         <f t="shared" si="1"/>
@@ -1895,27 +1888,27 @@
     </row>
     <row r="37" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="58">
-        <v>5324</v>
+        <v>5323</v>
       </c>
       <c r="B37" s="33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C37" s="33"/>
       <c r="D37" s="34"/>
-      <c r="E37" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="G37" s="37" t="s">
+      <c r="E37" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="F37" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="G37" s="48" t="s">
         <v>11</v>
       </c>
       <c r="H37" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I37" s="49">
-        <v>1.17</v>
+      <c r="I37" s="43">
+        <v>14.7</v>
       </c>
       <c r="J37" s="38">
         <f t="shared" si="1"/>
@@ -1924,25 +1917,27 @@
     </row>
     <row r="38" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="58">
-        <v>5328</v>
-      </c>
-      <c r="B38" s="39">
-        <v>2</v>
+        <v>5324</v>
+      </c>
+      <c r="B38" s="33">
+        <v>3</v>
       </c>
       <c r="C38" s="33"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="35">
-        <v>2860105462</v>
-      </c>
-      <c r="F38" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="G38" s="42"/>
-      <c r="H38" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="I38" s="43">
-        <v>1.85</v>
+      <c r="D38" s="34"/>
+      <c r="E38" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" s="49">
+        <v>1.17</v>
       </c>
       <c r="J38" s="38">
         <f t="shared" si="1"/>
@@ -1951,27 +1946,25 @@
     </row>
     <row r="39" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="58">
-        <v>5338</v>
+        <v>5328</v>
       </c>
       <c r="B39" s="39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C39" s="33"/>
       <c r="D39" s="40"/>
-      <c r="E39" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="F39" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="G39" s="42" t="s">
-        <v>46</v>
-      </c>
+      <c r="E39" s="35">
+        <v>2860105462</v>
+      </c>
+      <c r="F39" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="G39" s="42"/>
       <c r="H39" s="42" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="I39" s="43">
-        <v>286.66000000000003</v>
+        <v>1.85</v>
       </c>
       <c r="J39" s="38">
         <f t="shared" si="1"/>
@@ -1980,7 +1973,7 @@
     </row>
     <row r="40" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="58">
-        <v>5339</v>
+        <v>5338</v>
       </c>
       <c r="B40" s="39">
         <v>1</v>
@@ -1988,19 +1981,19 @@
       <c r="C40" s="33"/>
       <c r="D40" s="40"/>
       <c r="E40" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="F40" s="35" t="s">
-        <v>34</v>
+        <v>44</v>
+      </c>
+      <c r="F40" s="41" t="s">
+        <v>45</v>
       </c>
       <c r="G40" s="42" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="H40" s="42" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="I40" s="43">
-        <v>252.8</v>
+        <v>286.66000000000003</v>
       </c>
       <c r="J40" s="38">
         <f t="shared" si="1"/>
@@ -2009,7 +2002,7 @@
     </row>
     <row r="41" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="58">
-        <v>5340</v>
+        <v>5339</v>
       </c>
       <c r="B41" s="39">
         <v>1</v>
@@ -2017,10 +2010,10 @@
       <c r="C41" s="33"/>
       <c r="D41" s="40"/>
       <c r="E41" s="35" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F41" s="35" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="G41" s="42" t="s">
         <v>35</v>
@@ -2028,8 +2021,8 @@
       <c r="H41" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="I41" s="45">
-        <v>6.13</v>
+      <c r="I41" s="43">
+        <v>252.8</v>
       </c>
       <c r="J41" s="38">
         <f t="shared" si="1"/>
@@ -2038,27 +2031,27 @@
     </row>
     <row r="42" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="58">
-        <v>5341</v>
-      </c>
-      <c r="B42" s="33">
+        <v>5340</v>
+      </c>
+      <c r="B42" s="39">
         <v>1</v>
       </c>
       <c r="C42" s="33"/>
-      <c r="D42" s="34"/>
+      <c r="D42" s="40"/>
       <c r="E42" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="F42" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="G42" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="H42" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="I42" s="43">
-        <v>11.25</v>
+        <v>37</v>
+      </c>
+      <c r="F42" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="H42" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="I42" s="45">
+        <v>6.13</v>
       </c>
       <c r="J42" s="38">
         <f t="shared" si="1"/>
@@ -2067,27 +2060,27 @@
     </row>
     <row r="43" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="58">
-        <v>5342</v>
-      </c>
-      <c r="B43" s="39">
+        <v>5341</v>
+      </c>
+      <c r="B43" s="33">
         <v>1</v>
       </c>
       <c r="C43" s="33"/>
-      <c r="D43" s="40"/>
+      <c r="D43" s="34"/>
       <c r="E43" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="F43" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="G43" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="H43" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="I43" s="52">
-        <v>13.85</v>
+        <v>26</v>
+      </c>
+      <c r="F43" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="G43" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="H43" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="I43" s="43">
+        <v>11.25</v>
       </c>
       <c r="J43" s="38">
         <f t="shared" si="1"/>
@@ -2096,7 +2089,7 @@
     </row>
     <row r="44" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="58">
-        <v>5343</v>
+        <v>5342</v>
       </c>
       <c r="B44" s="39">
         <v>1</v>
@@ -2104,10 +2097,10 @@
       <c r="C44" s="33"/>
       <c r="D44" s="40"/>
       <c r="E44" s="35" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="F44" s="35" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="G44" s="42" t="s">
         <v>49</v>
@@ -2115,10 +2108,39 @@
       <c r="H44" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="I44" s="43">
+      <c r="I44" s="52">
+        <v>13.85</v>
+      </c>
+      <c r="J44" s="38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" s="4" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="58">
+        <v>5343</v>
+      </c>
+      <c r="B45" s="39">
+        <v>1</v>
+      </c>
+      <c r="C45" s="33"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="F45" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="G45" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="H45" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="I45" s="43">
         <v>8.74</v>
       </c>
-      <c r="J44" s="38">
+      <c r="J45" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2128,7 +2150,7 @@
     <sortCondition ref="A9"/>
   </sortState>
   <mergeCells count="6">
-    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="A2:D2"/>

</xml_diff>